<commit_message>
Regenerate documents with updated level-of-effort estimates and refine presales artifacts
Updated level-of-effort CSV files and regenerated all output documents for both solution-template and intelligent-document-processing. Replaced outdated presales documents (business-case, executive-presentation, requirements-questionnaire, roi-calculator) with streamlined artifacts (discovery-questionnaire, solution-briefing). Enhanced statement-of-work with expanded content and improved template generation scripts.
</commit_message>
<xml_diff>
--- a/solution-template/sample-provider/sample-category/sample-solution/delivery/communication-plan.xlsx
+++ b/solution-template/sample-provider/sample-category/sample-solution/delivery/communication-plan.xlsx
@@ -207,10 +207,10 @@
     <from>
       <col>1</col>
       <colOff>0</colOff>
-      <row>2</row>
+      <row>14</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1428750" cy="476250"/>
+    <ext cx="1143000" cy="285750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -218,62 +218,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>12</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1428750" cy="476250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>14</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="1905000" cy="476250"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -595,7 +539,7 @@
   <sheetData>
     <row r="1" ht="20" customHeight="1"/>
     <row r="2" ht="10" customHeight="1"/>
-    <row r="3" ht="60" customHeight="1"/>
+    <row r="3" ht="20" customHeight="1"/>
     <row r="4" ht="30" customHeight="1">
       <c r="B4" s="1" t="inlineStr">
         <is>
@@ -638,7 +582,7 @@
     <row r="9">
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Purpose:</t>
+          <t>Customer Name:</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
@@ -661,9 +605,9 @@
     </row>
     <row r="11" ht="20" customHeight="1"/>
     <row r="12" ht="10" customHeight="1"/>
-    <row r="13" ht="60" customHeight="1"/>
+    <row r="13" ht="10" customHeight="1"/>
     <row r="14" ht="10" customHeight="1"/>
-    <row r="15" ht="60" customHeight="1"/>
+    <row r="15" ht="40" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Update solution template - consolidate Investment Summary structure and optimize table formatting
</commit_message>
<xml_diff>
--- a/solution-template/sample-provider/sample-category/sample-solution/delivery/communication-plan.xlsx
+++ b/solution-template/sample-provider/sample-category/sample-solution/delivery/communication-plan.xlsx
@@ -563,7 +563,7 @@
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t>November 11, 2025</t>
+          <t>November 15, 2025</t>
         </is>
       </c>
     </row>
@@ -1055,7 +1055,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="26" customHeight="1">
+    <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
           <t>COMM-005</t>
@@ -1137,7 +1137,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="26" customHeight="1">
+    <row r="7">
       <c r="A7" s="7" t="inlineStr">
         <is>
           <t>COMM-006</t>
@@ -1219,7 +1219,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="26" customHeight="1">
+    <row r="8">
       <c r="A8" s="6" t="inlineStr">
         <is>
           <t>COMM-007</t>
@@ -1301,7 +1301,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="26" customHeight="1">
+    <row r="9">
       <c r="A9" s="7" t="inlineStr">
         <is>
           <t>COMM-008</t>
@@ -1383,7 +1383,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="26" customHeight="1">
+    <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
           <t>COMM-009</t>
@@ -1465,7 +1465,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="26" customHeight="1">
+    <row r="11">
       <c r="A11" s="7" t="inlineStr">
         <is>
           <t>COMM-010</t>
@@ -1547,7 +1547,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="26" customHeight="1">
+    <row r="12">
       <c r="A12" s="6" t="inlineStr">
         <is>
           <t>COMM-011</t>
@@ -1629,7 +1629,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="26" customHeight="1">
+    <row r="13">
       <c r="A13" s="7" t="inlineStr">
         <is>
           <t>COMM-012</t>
@@ -1711,7 +1711,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="26" customHeight="1">
+    <row r="14">
       <c r="A14" s="6" t="inlineStr">
         <is>
           <t>COMM-013</t>
@@ -1793,7 +1793,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="26" customHeight="1">
+    <row r="15">
       <c r="A15" s="7" t="inlineStr">
         <is>
           <t>COMM-014</t>
@@ -1875,7 +1875,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="26" customHeight="1">
+    <row r="16">
       <c r="A16" s="6" t="inlineStr">
         <is>
           <t>COMM-015</t>
@@ -1957,7 +1957,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="26" customHeight="1">
+    <row r="17">
       <c r="A17" s="7" t="inlineStr">
         <is>
           <t>COMM-016</t>
@@ -2039,7 +2039,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="26" customHeight="1">
+    <row r="18">
       <c r="A18" s="6" t="inlineStr">
         <is>
           <t>COMM-017</t>
@@ -2121,7 +2121,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="26" customHeight="1">
+    <row r="19">
       <c r="A19" s="7" t="inlineStr">
         <is>
           <t>COMM-018</t>
@@ -2203,7 +2203,7 @@
         </is>
       </c>
     </row>
-    <row r="20" ht="26" customHeight="1">
+    <row r="20">
       <c r="A20" s="6" t="inlineStr">
         <is>
           <t>COMM-019</t>
@@ -2285,7 +2285,7 @@
         </is>
       </c>
     </row>
-    <row r="21" ht="26" customHeight="1">
+    <row r="21">
       <c r="A21" s="7" t="inlineStr">
         <is>
           <t>COMM-020</t>

</xml_diff>